<commit_message>
adding project batch upload
</commit_message>
<xml_diff>
--- a/Project-Export.xlsx
+++ b/Project-Export.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mayayaradena/Documents/DEV/DB_kecamatan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BBFFAC14-01D4-FE46-B749-C6CA7E0174AB}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D7E5BD87-6A06-C04D-9787-5BB084034A10}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -2116,8 +2116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X2" sqref="X2:X20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3686,7 +3686,7 @@
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>KAMUS!$C$3:$C$5</xm:f>
@@ -3699,17 +3699,11 @@
           </x14:formula1>
           <xm:sqref>O2:O20</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A094532D-8CB5-7D44-A9C3-A3B1A1C15355}">
-          <x14:formula1>
-            <xm:f>KAMUS!$B$4:$B$8</xm:f>
-          </x14:formula1>
-          <xm:sqref>C3:C20</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{68C493E2-5C19-4241-8705-1FC8FC20BC54}">
           <x14:formula1>
             <xm:f>KAMUS!$B$3:$B$8</xm:f>
           </x14:formula1>
-          <xm:sqref>C2</xm:sqref>
+          <xm:sqref>C2:C20</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3721,7 +3715,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:F508"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>

</xml_diff>